<commit_message>
_04_ Runner Plugin has beed added for extent report & corrected POM root
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/CampusReport.xlsx
+++ b/src/test/java/ApachePOI/Resources/CampusReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="176">
   <si>
     <t>f934faee-2c94-4c2b-b933-8c1017a07889</t>
   </si>
@@ -524,6 +524,30 @@
   </si>
   <si>
     <t>PT18.9629597S</t>
+  </si>
+  <si>
+    <t>04c80963-c1da-46a9-beb6-4133d0481392</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_01_59</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_02_05</t>
+  </si>
+  <si>
+    <t>PT5.3599447S</t>
+  </si>
+  <si>
+    <t>4b04eaf8-8f23-42b1-8c34-0e8c0196e588</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_02_09</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_02_16</t>
+  </si>
+  <si>
+    <t>PT7.2188974S</t>
   </si>
 </sst>
 </file>
@@ -879,7 +903,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -2234,6 +2258,46 @@
         <v>167</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s" s="1">
+        <v>169</v>
+      </c>
+      <c r="E68" t="s" s="1">
+        <v>170</v>
+      </c>
+      <c r="F68" t="s" s="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s" s="1">
+        <v>173</v>
+      </c>
+      <c r="E69" t="s" s="1">
+        <v>174</v>
+      </c>
+      <c r="F69" t="s" s="1">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chrome option added for Jenkins
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/CampusReport.xlsx
+++ b/src/test/java/ApachePOI/Resources/CampusReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="194">
   <si>
     <t>f934faee-2c94-4c2b-b933-8c1017a07889</t>
   </si>
@@ -548,6 +548,60 @@
   </si>
   <si>
     <t>PT7.2188974S</t>
+  </si>
+  <si>
+    <t>ae36fa6e-f222-4071-aec0-1c31450a4470</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_53_58</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_06</t>
+  </si>
+  <si>
+    <t>PT8.3587541S</t>
+  </si>
+  <si>
+    <t>4b08957a-055f-48e6-8ec5-01493c4c5f9e</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_11</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_19</t>
+  </si>
+  <si>
+    <t>PT8.0514124S</t>
+  </si>
+  <si>
+    <t>2958d93b-e068-4570-8ae0-9059f8fff0cb</t>
+  </si>
+  <si>
+    <t>Create country with parameters</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_22</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_31</t>
+  </si>
+  <si>
+    <t>PT8.6318558S</t>
+  </si>
+  <si>
+    <t>adf99497-3ed2-4980-9f65-2c598b736c6b</t>
+  </si>
+  <si>
+    <t>Delete country with parameters</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_34</t>
+  </si>
+  <si>
+    <t>03_28_2024_19_54_42</t>
+  </si>
+  <si>
+    <t>PT7.9847116S</t>
   </si>
 </sst>
 </file>
@@ -903,7 +957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -2298,6 +2352,86 @@
         <v>175</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s" s="1">
+        <v>177</v>
+      </c>
+      <c r="E70" t="s" s="1">
+        <v>178</v>
+      </c>
+      <c r="F70" t="s" s="1">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s" s="1">
+        <v>181</v>
+      </c>
+      <c r="E71" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="F71" t="s" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s" s="1">
+        <v>186</v>
+      </c>
+      <c r="E72" t="s" s="1">
+        <v>187</v>
+      </c>
+      <c r="F72" t="s" s="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s" s="1">
+        <v>191</v>
+      </c>
+      <c r="E73" t="s" s="1">
+        <v>192</v>
+      </c>
+      <c r="F73" t="s" s="1">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected plugins for Jenkins Cucumber report
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/CampusReport.xlsx
+++ b/src/test/java/ApachePOI/Resources/CampusReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="202">
   <si>
     <t>f934faee-2c94-4c2b-b933-8c1017a07889</t>
   </si>
@@ -602,6 +602,30 @@
   </si>
   <si>
     <t>PT7.9847116S</t>
+  </si>
+  <si>
+    <t>31b57bd0-6c05-41b5-8f14-48622428d41d</t>
+  </si>
+  <si>
+    <t>03_28_2024_22_55_57</t>
+  </si>
+  <si>
+    <t>03_28_2024_22_56_08</t>
+  </si>
+  <si>
+    <t>PT11.1655475S</t>
+  </si>
+  <si>
+    <t>8c06243c-0e6f-4b2d-852c-38835e66d1ea</t>
+  </si>
+  <si>
+    <t>03_28_2024_22_56_13</t>
+  </si>
+  <si>
+    <t>03_28_2024_22_56_24</t>
+  </si>
+  <si>
+    <t>PT10.9984168S</t>
   </si>
 </sst>
 </file>
@@ -957,7 +981,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -2432,6 +2456,46 @@
         <v>193</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s" s="1">
+        <v>195</v>
+      </c>
+      <c r="E74" t="s" s="1">
+        <v>196</v>
+      </c>
+      <c r="F74" t="s" s="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C75" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s" s="1">
+        <v>199</v>
+      </c>
+      <c r="E75" t="s" s="1">
+        <v>200</v>
+      </c>
+      <c r="F75" t="s" s="1">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Runner class updated plugin
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/CampusReport.xlsx
+++ b/src/test/java/ApachePOI/Resources/CampusReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="210">
   <si>
     <t>f934faee-2c94-4c2b-b933-8c1017a07889</t>
   </si>
@@ -626,6 +626,30 @@
   </si>
   <si>
     <t>PT10.9984168S</t>
+  </si>
+  <si>
+    <t>65840174-3784-43b7-86fe-cfe855126c5e</t>
+  </si>
+  <si>
+    <t>03_29_2024_00_15_59</t>
+  </si>
+  <si>
+    <t>03_29_2024_00_16_05</t>
+  </si>
+  <si>
+    <t>PT5.90775S</t>
+  </si>
+  <si>
+    <t>c11cb73a-64df-47c9-be4c-b157d0f70c74</t>
+  </si>
+  <si>
+    <t>03_29_2024_00_16_09</t>
+  </si>
+  <si>
+    <t>03_29_2024_00_16_17</t>
+  </si>
+  <si>
+    <t>PT8.3585238S</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1005,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -2496,6 +2520,46 @@
         <v>201</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s" s="1">
+        <v>203</v>
+      </c>
+      <c r="E76" t="s" s="1">
+        <v>204</v>
+      </c>
+      <c r="F76" t="s" s="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C77" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s" s="1">
+        <v>207</v>
+      </c>
+      <c r="E77" t="s" s="1">
+        <v>208</v>
+      </c>
+      <c r="F77" t="s" s="1">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>